<commit_message>
Modified production files for jclpcb
</commit_message>
<xml_diff>
--- a/8-Solenoid-PCB/Project Outputs for 8-Solenoid-Board/8-Solenoid-Board-BOM.xlsx
+++ b/8-Solenoid-PCB/Project Outputs for 8-Solenoid-Board/8-Solenoid-Board-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/jl83722_my_utexas_edu/Documents/00 - UT Austin/Orgs/Momentum/Altium/8-Solenoid-PCB/Project Outputs for 8-Solenoid-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{4C8EA619-4685-4748-BAF8-C1BF9E25E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46E4595C-375E-49A1-AB07-B0DFC3EC1E5E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{4C8EA619-4685-4748-BAF8-C1BF9E25E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74EF46FB-3582-4273-B397-EF0445F686C6}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{2A26D8B6-A346-451E-B790-108E80C3A65A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Comment</t>
   </si>
@@ -77,16 +77,7 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Mfg Part #</t>
-  </si>
-  <si>
     <t>Diodes</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>SMD</t>
   </si>
 </sst>
 </file>
@@ -143,12 +134,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -165,6 +157,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,18 +480,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58291281-9555-4D98-A1FF-CEF096166EEE}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="19" customWidth="1"/>
+    <col min="1" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -509,22 +505,17 @@
         <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -535,89 +526,28 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="G2" s="1">
         <v>8</v>
       </c>
+      <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>